<commit_message>
sửa lại phép trừ
</commit_message>
<xml_diff>
--- a/salary2.xlsx
+++ b/salary2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\Môn thực tập ngành\end\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\bigInt-algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2EB01E-572A-4B2A-9256-B85C50E063C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ADE85D-0D1B-4113-938C-D7C9440A65A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9015" yWindow="2640" windowWidth="13755" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>index</t>
   </si>
@@ -31,46 +31,67 @@
     <t>salary</t>
   </si>
   <si>
-    <t>Trần Văn A</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị B</t>
-  </si>
-  <si>
-    <t>Lê Thị C</t>
-  </si>
-  <si>
-    <t>Phạm Văn D</t>
-  </si>
-  <si>
-    <t>Lê Thị E</t>
-  </si>
-  <si>
-    <t>Nguyễn Kim F</t>
-  </si>
-  <si>
-    <t>Đào Văn L</t>
-  </si>
-  <si>
-    <t>Phạm Thị N</t>
-  </si>
-  <si>
-    <t>Lê Tuấn M</t>
-  </si>
-  <si>
-    <t>Nguyễn Duy C</t>
-  </si>
-  <si>
-    <t>Lê Thị L</t>
+    <t>Nguyễn Bảo Ngọc</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Hùng</t>
+  </si>
+  <si>
+    <t>Lê Anh Hoà</t>
+  </si>
+  <si>
+    <t>Vũ Thị Thủy</t>
+  </si>
+  <si>
+    <t>Nguyễn Huệ Ánh</t>
+  </si>
+  <si>
+    <t>Phạm Văn Thanh</t>
+  </si>
+  <si>
+    <t>Võ Minh Sang</t>
+  </si>
+  <si>
+    <t>Nguyễn Đình Hoàng Sơn</t>
+  </si>
+  <si>
+    <t>Trần Thái Tài</t>
+  </si>
+  <si>
+    <t>Nguyễn Xuân Thành</t>
+  </si>
+  <si>
+    <t>Lê Tấn Đạt</t>
+  </si>
+  <si>
+    <t>Nguyễn Thành Đạt</t>
+  </si>
+  <si>
+    <t>Nguyễn Hữu Lê Tuấn</t>
+  </si>
+  <si>
+    <t>Vũ Văn Tú</t>
+  </si>
+  <si>
+    <t>Thiều Minh Trường</t>
+  </si>
+  <si>
+    <t>Nguyễn Đức Trọng</t>
+  </si>
+  <si>
+    <t>Nguyễn Đức Thành Nhân</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Hồng Châu</t>
+  </si>
+  <si>
+    <t>Điểu Phan Quang Anh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00\ [$đ-42A]"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -105,10 +126,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -327,52 +349,54 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="36.44140625" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2">
-        <v>2334567</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>233456789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>2334567</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>233456789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -380,76 +404,76 @@
         <v>5</v>
       </c>
       <c r="C4" s="2">
-        <v>2334567</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>233456789</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
-        <v>2334567</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>233456789</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2">
-        <v>2334567</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>233456789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2">
-        <v>2334567</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2">
-        <v>2334567</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2">
-        <v>2334567</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2">
-        <v>2334567</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -457,10 +481,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="2">
-        <v>2334567</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -468,10 +492,99 @@
         <v>13</v>
       </c>
       <c r="C12" s="2">
-        <v>2334567</v>
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="2">
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2">
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="2">
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2">
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="2">
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="2">
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2">
+        <v>12334567891011</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="2">
+        <v>12334567891011</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>